<commit_message>
Week 10 - Sprint
Added my section to the Sprint
</commit_message>
<xml_diff>
--- a/Documents/Burndownchart.xlsx
+++ b/Documents/Burndownchart.xlsx
@@ -561,10 +561,10 @@
                   <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>54</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>54</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1650,7 +1650,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+      <selection activeCell="C17" sqref="C17:L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1818,7 +1818,7 @@
       </c>
       <c r="D11" s="1">
         <f>K32</f>
-        <v>54</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="D12" s="1">
         <f>L32</f>
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1913,7 +1913,7 @@
         <v>9</v>
       </c>
       <c r="M17" s="1">
-        <f t="shared" ref="M17:M23" si="0">SUM(C17:J17)/B17*100</f>
+        <f>SUM(C17:L17)/B17*100</f>
         <v>100</v>
       </c>
     </row>
@@ -1940,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="M18:M30" si="0">SUM(C18:L18)/B18*100</f>
         <v>100</v>
       </c>
     </row>
@@ -2062,9 +2062,12 @@
       <c r="J24" s="1">
         <v>9</v>
       </c>
+      <c r="K24" s="1">
+        <v>9</v>
+      </c>
       <c r="M24" s="1">
-        <f t="shared" ref="M24:M30" si="1">SUM(C24:J24)/B24*100</f>
-        <v>66.666666666666657</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -2078,7 +2081,7 @@
         <v>9</v>
       </c>
       <c r="M25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -2093,7 +2096,7 @@
         <v>9</v>
       </c>
       <c r="M26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -2107,9 +2110,12 @@
       <c r="J27" s="1">
         <v>9</v>
       </c>
+      <c r="K27" s="1">
+        <v>9</v>
+      </c>
       <c r="M27" s="1">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -2119,9 +2125,15 @@
       <c r="B28" s="1">
         <v>18</v>
       </c>
+      <c r="K28" s="1">
+        <v>9</v>
+      </c>
+      <c r="L28" s="1">
+        <v>9</v>
+      </c>
       <c r="M28" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -2134,9 +2146,12 @@
       <c r="J29" s="1">
         <v>9</v>
       </c>
+      <c r="K29" s="1">
+        <v>9</v>
+      </c>
       <c r="M29" s="1">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -2146,9 +2161,12 @@
       <c r="B30" s="1">
         <v>9</v>
       </c>
+      <c r="L30" s="1">
+        <v>9</v>
+      </c>
       <c r="M30" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -2196,44 +2214,44 @@
         <v>306</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" ref="C32:L32" si="2">B32-SUM(C17:C30)</f>
+        <f t="shared" ref="C32:L32" si="1">B32-SUM(C17:C30)</f>
         <v>306</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>270</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>234</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>204</v>
       </c>
       <c r="G32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>177</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>135</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" si="2"/>
-        <v>54</v>
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
       <c r="L32" s="1">
-        <f t="shared" si="2"/>
-        <v>54</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>